<commit_message>
AWS bash cmd line
</commit_message>
<xml_diff>
--- a/bbCeny.xlsx
+++ b/bbCeny.xlsx
@@ -465,7 +465,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Last status check on: 07.01.2022 15:17</t>
+          <t>Last status check on: 07.01.2022 15:18</t>
         </is>
       </c>
     </row>
@@ -481,15 +481,11 @@
       <c r="C2" t="n">
         <v>32.9</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>+0.6</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2022-01-07 15:17:06</t>
-        </is>
+      <c r="D2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>44568.636875</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>

</xml_diff>